<commit_message>
updated small benchmark results
</commit_message>
<xml_diff>
--- a/fse-benchmark-results.xlsx
+++ b/fse-benchmark-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Benchmark Program</t>
   </si>
@@ -56,12 +56,36 @@
   <si>
     <t>ems-hashtest</t>
   </si>
+  <si>
+    <t>std-cryptobench</t>
+  </si>
+  <si>
+    <t>opn-linq_functional</t>
+  </si>
+  <si>
+    <t>opn-linq_aggregate</t>
+  </si>
+  <si>
+    <t>opn-linq_dictionary</t>
+  </si>
+  <si>
+    <t>opn-linq_enumerable</t>
+  </si>
+  <si>
+    <t>1-cfa argument-sensitive overall points-to size</t>
+  </si>
+  <si>
+    <t>diagnostic-cfa argument-sensitive overall points-to size</t>
+  </si>
+  <si>
+    <t>0-1-cfa argument-sensitive overall points-to size</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +109,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +135,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -117,23 +149,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -182,7 +227,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$119</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>ems-fourinarow</c:v>
                 </c:pt>
@@ -203,6 +248,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -233,6 +293,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2798.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8827.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2775.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3036.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2497.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3380.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,7 +335,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$119</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>ems-fourinarow</c:v>
                 </c:pt>
@@ -281,6 +356,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -311,6 +401,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2563.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7624.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2144.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2182.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2231.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3063.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,9 +525,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>ems-fourinarow</c:v>
                 </c:pt>
@@ -443,16 +548,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>6344.0</c:v>
                 </c:pt>
@@ -473,6 +593,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2798.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8827.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2775.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3036.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2497.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3380.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,9 +630,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>ems-fourinarow</c:v>
                 </c:pt>
@@ -518,16 +653,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5296.0</c:v>
                 </c:pt>
@@ -548,6 +698,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2563.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7624.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2144.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2182.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2231.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3063.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -570,9 +735,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>ems-fourinarow</c:v>
                 </c:pt>
@@ -593,16 +758,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5753.0</c:v>
                 </c:pt>
@@ -623,6 +803,126 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2660.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7849.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2707.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2635.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2324.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3303.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no. of diagnostic functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>ems-fourinarow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ems-aha</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ems-fasta</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ems-sgefa</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ems-llubenchmark</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ems-fannkuch</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ems-hashtest</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>std-cryptobench</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>opn-linq_enumerable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,11 +937,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2113222648"/>
-        <c:axId val="2097848360"/>
+        <c:axId val="2112503352"/>
+        <c:axId val="2116385528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113222648"/>
+        <c:axId val="2112503352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097848360"/>
+        <c:crossAx val="2116385528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -658,7 +958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097848360"/>
+        <c:axId val="2116385528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +969,262 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113222648"/>
+        <c:crossAx val="2112503352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0-1-cfa argument-sensitive overall points-to size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>opn-linq_enumerable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2775.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3036.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2497.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3380.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1-cfa argument-sensitive overall points-to size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>opn-linq_enumerable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2084.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2166.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2198.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2702.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>diagnostic-cfa argument-sensitive overall points-to size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>opn-linq_functional</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>opn-linq_aggregate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>opn-linq_dictionary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>opn-linq_enumerable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2353.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2376.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2255.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2813.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2137981608"/>
+        <c:axId val="2118757432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2137981608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118757432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118757432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137981608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -725,20 +1280,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -748,6 +1303,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1955800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1078,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1091,13 +1676,17 @@
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="7" max="7" width="0.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" customWidth="1"/>
+    <col min="7" max="7" width="4.5" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" customWidth="1"/>
     <col min="10" max="10" width="31.83203125" customWidth="1"/>
+    <col min="11" max="11" width="46.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.1640625" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +1702,23 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1130,8 +1734,23 @@
       <c r="E2">
         <v>11</v>
       </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>2775</v>
+      </c>
+      <c r="K2">
+        <v>2084</v>
+      </c>
+      <c r="L2">
+        <v>2353</v>
+      </c>
+      <c r="M2">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1147,8 +1766,23 @@
       <c r="E3">
         <v>5</v>
       </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>3036</v>
+      </c>
+      <c r="K3">
+        <v>2166</v>
+      </c>
+      <c r="L3">
+        <v>2376</v>
+      </c>
+      <c r="M3">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1164,8 +1798,23 @@
       <c r="E4">
         <v>7</v>
       </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>2497</v>
+      </c>
+      <c r="K4">
+        <v>2198</v>
+      </c>
+      <c r="L4">
+        <v>2255</v>
+      </c>
+      <c r="M4">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1181,8 +1830,23 @@
       <c r="E5">
         <v>8</v>
       </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>3380</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2702</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2813</v>
+      </c>
+      <c r="M5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1199,7 +1863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1231,6 +1895,91 @@
       </c>
       <c r="E8">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>8827</v>
+      </c>
+      <c r="C10">
+        <v>7624</v>
+      </c>
+      <c r="D10">
+        <v>7849</v>
+      </c>
+      <c r="E10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2775</v>
+      </c>
+      <c r="C12">
+        <v>2144</v>
+      </c>
+      <c r="D12">
+        <v>2707</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>3036</v>
+      </c>
+      <c r="C13">
+        <v>2182</v>
+      </c>
+      <c r="D13">
+        <v>2635</v>
+      </c>
+      <c r="E13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>2497</v>
+      </c>
+      <c r="C14">
+        <v>2231</v>
+      </c>
+      <c r="D14">
+        <v>2324</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>3380</v>
+      </c>
+      <c r="C15">
+        <v>3063</v>
+      </c>
+      <c r="D15">
+        <v>3303</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>